<commit_message>
documentacao do procedimento de calculo para as calorias (cap. do relatorio)
</commit_message>
<xml_diff>
--- a/others/calorias.xlsx
+++ b/others/calorias.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="9555" windowHeight="6465" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="9555" windowHeight="6465"/>
   </bookViews>
   <sheets>
     <sheet name="HR" sheetId="1" r:id="rId1"/>
     <sheet name="CPA" sheetId="2" r:id="rId2"/>
-    <sheet name="Folha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="BMRh">HR!$C$11</definedName>
@@ -62,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="71">
   <si>
     <t>Peso</t>
   </si>
@@ -574,6 +573,30 @@
   </si>
   <si>
     <t>BC</t>
+  </si>
+  <si>
+    <r>
+      <t>Ainsworth BE, Haskell WL, Herrmann SD, Meckes N, Bassett Jr DR, Tudor-Locke C, Greer JL, Vezina J, Whitt-    Glover MC, Leon AS. 2011 Compendium of Physical Activities: a second update of codes and MET values. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Medicine and Science in Sports and Exercise</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 2011;43(8):1575-1581.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -581,9 +604,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -630,6 +653,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -663,7 +699,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -671,8 +707,9 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1036,8 +1073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1322,10 +1359,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:A31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,22 +1370,25 @@
     <col min="2" max="2" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -1356,7 +1396,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1367,7 +1407,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1375,7 +1415,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1383,7 +1423,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1391,7 +1431,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1399,7 +1439,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1407,7 +1447,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1418,7 +1458,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1426,7 +1466,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1437,7 +1477,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -1445,7 +1485,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1456,7 +1496,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -1631,18 +1671,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>